<commit_message>
products added to the sheet
</commit_message>
<xml_diff>
--- a/work_book_1.xlsx
+++ b/work_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00F059A0-BE99-482D-BEC3-CB6EE6C8746A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E39B41-03BC-46CD-84AD-1C13BC0A8785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74BCC72C-4CB7-45E2-B286-F8BEF58EF335}"/>
   </bookViews>
@@ -32,9 +32,78 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>WalMArt</t>
+  </si>
+  <si>
+    <t>Dollar Trap</t>
+  </si>
+  <si>
+    <t>Office Repo</t>
+  </si>
+  <si>
+    <t>Ball Point Pen</t>
+  </si>
+  <si>
+    <t>TI-35 Calculator</t>
+  </si>
+  <si>
+    <t>100 Page Notebook</t>
+  </si>
+  <si>
+    <t>8 oz Glue</t>
+  </si>
+  <si>
+    <t>Clear Tape</t>
+  </si>
+  <si>
+    <t>Eraser</t>
+  </si>
+  <si>
+    <t>10 No.2 Pencils</t>
+  </si>
+  <si>
+    <t>2inch Binder</t>
+  </si>
+  <si>
+    <t>USB Stick 5gb</t>
+  </si>
+  <si>
+    <t>Color Markers</t>
+  </si>
+  <si>
+    <t>Stapler</t>
+  </si>
+  <si>
+    <t>Planner Book</t>
+  </si>
+  <si>
+    <t>Protractor</t>
+  </si>
+  <si>
+    <t>Compass</t>
+  </si>
+  <si>
+    <t>Liquid Paper</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +129,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,12 +454,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEFB44C-F5F5-4CBD-8D35-04C92DE5A776}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.55</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
calculated the total amount spent by susan for each store
</commit_message>
<xml_diff>
--- a/work_book_1.xlsx
+++ b/work_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E39B41-03BC-46CD-84AD-1C13BC0A8785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A233A2-8ED6-411A-AA8C-FDD613FBDE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74BCC72C-4CB7-45E2-B286-F8BEF58EF335}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>WalMArt</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Liquid Paper</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -133,12 +142,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -454,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEFB44C-F5F5-4CBD-8D35-04C92DE5A776}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -473,8 +484,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -487,8 +513,23 @@
       <c r="D2" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4">
+        <f>$F2*B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2:J2" si="0">$F2*C2</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J2" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -501,8 +542,23 @@
       <c r="D3" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H15" si="1">$F3*B3</f>
+        <v>28</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I15" si="2">$F3*C3</f>
+        <v>33</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J15" si="3">$F3*D3</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -515,8 +571,23 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="1"/>
+        <v>12.6</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -529,8 +600,23 @@
       <c r="D5" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -543,8 +629,23 @@
       <c r="D6" s="2">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="1"/>
+        <v>4.8</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="2"/>
+        <v>2.8</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="3"/>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -557,8 +658,23 @@
       <c r="D7" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="3"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -571,8 +687,23 @@
       <c r="D8" s="2">
         <v>2.59</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.59</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="3"/>
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -585,8 +716,23 @@
       <c r="D9" s="2">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="3"/>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -599,8 +745,23 @@
       <c r="D10" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -613,8 +774,23 @@
       <c r="D11" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="1"/>
+        <v>4.55</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="2"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -627,8 +803,23 @@
       <c r="D12" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -641,8 +832,23 @@
       <c r="D13" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -655,8 +861,23 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -669,8 +890,23 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -682,6 +918,23 @@
       </c>
       <c r="D16" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="4">
+        <f>SUM(H2:H15)</f>
+        <v>80.790000000000006</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" ref="I17:J17" si="4">SUM(I2:I15)</f>
+        <v>86.539999999999992</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="4"/>
+        <v>100.28999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created graph according to the totoal money spent
</commit_message>
<xml_diff>
--- a/work_book_1.xlsx
+++ b/work_book_1.xlsx
@@ -8,13 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A233A2-8ED6-411A-AA8C-FDD613FBDE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6056FFAD-51F7-40EA-887D-5C0F95383131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74BCC72C-4CB7-45E2-B286-F8BEF58EF335}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$H$17:$J$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -155,7 +168,38 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -166,6 +210,689 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Total </cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Total </a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{92D3659E-DE02-4B66-B84E-430CE817812D}">
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="388">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>380999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BABB336-E99A-F65F-525C-48C798E5BEFE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="380999"/>
+              <a:ext cx="3381375" cy="2581275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -468,7 +1195,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,6 +1665,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H17:J17">
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
claculated the money spent by Tim and created the graph according to the expense
</commit_message>
<xml_diff>
--- a/work_book_1.xlsx
+++ b/work_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6056FFAD-51F7-40EA-887D-5C0F95383131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70641D3D-497A-4E62-8612-5DA268394882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74BCC72C-4CB7-45E2-B286-F8BEF58EF335}"/>
   </bookViews>
@@ -16,12 +16,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$H$17:$J$17</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$N$17</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$1:$J$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$17:$J$17</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$H$1:$J$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$N$17</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$O$17:$Q$17</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$H$1:$J$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$N$17</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$O$17:$Q$17</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$O$17:$Q$17</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$H$17:$J$17</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$H$1:$J$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$17:$J$17</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1:$J$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$17:$J$17</definedName>
@@ -46,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>WalMArt</t>
   </si>
@@ -109,6 +114,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Total Sum</t>
   </si>
 </sst>
 </file>
@@ -217,10 +228,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.v1.0</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -268,7 +279,109 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Total </cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Total </a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{5F2E6A25-2122-48AD-969C-1C112F007B2B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:v>Total Sum</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -812,20 +925,524 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="388">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>380999</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -861,8 +1478,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="380999"/>
+              <a:off x="0" y="1409699"/>
               <a:ext cx="3381375" cy="2581275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5C29739-D9DE-2E6E-CCC4-59C8CBD3CED9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8915400" y="1724025"/>
+              <a:ext cx="4267200" cy="2352675"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1192,15 +1887,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEFB44C-F5F5-4CBD-8D35-04C92DE5A776}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H19" activeCellId="1" sqref="O17:Q17 H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1226,8 +1921,23 @@
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1255,8 +1965,24 @@
         <f t="shared" si="0"/>
         <v>4.1999999999999993</v>
       </c>
+      <c r="M2" s="3">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4">
+        <f>B2*$M2</f>
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <f t="shared" ref="P2:Q2" si="1">C2*$M2</f>
+        <v>0.8</v>
+      </c>
+      <c r="Q2" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1273,19 +1999,34 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H15" si="1">$F3*B3</f>
+        <f t="shared" ref="H3:H15" si="2">$F3*B3</f>
         <v>28</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I15" si="2">$F3*C3</f>
+        <f t="shared" ref="I3:I15" si="3">$F3*C3</f>
         <v>33</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:J15" si="3">$F3*D3</f>
+        <f t="shared" ref="J3:J15" si="4">$F3*D3</f>
         <v>31</v>
       </c>
+      <c r="M3" s="3">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:O15" si="5">B3*$M3</f>
+        <v>56</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P15" si="6">C3*$M3</f>
+        <v>66</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q15" si="7">D3*$M3</f>
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1302,193 +2043,298 @@
         <v>7</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.6</v>
       </c>
       <c r="I4" s="4">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="5"/>
+        <v>1.8</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
+        <v>1.2</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="6"/>
+        <v>0.8</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4">
+      <c r="B6" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="2"/>
+        <v>4.8</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="4"/>
+        <v>4.8</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
+        <v>2.4</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="6"/>
+        <v>1.4</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.8</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.9</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.59</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.59</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="4"/>
+        <v>2.59</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="6"/>
+        <v>1.77</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="7"/>
+        <v>7.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="4"/>
+        <v>8.6</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="5"/>
+        <v>1.25</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="6"/>
+        <v>3.25</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="7"/>
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+      <c r="I10" s="4">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
+      <c r="J10" s="4">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="M10" s="3">
+        <v>8</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="6"/>
+        <v>112</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="7"/>
+        <v>104</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>4.8</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="3"/>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>1.8</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="3"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.99</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.59</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.59</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>0.59</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="3"/>
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3.25</v>
-      </c>
-      <c r="D9" s="2">
-        <v>2.15</v>
-      </c>
-      <c r="F9" s="3">
-        <v>4</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="3"/>
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2">
-        <v>13</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>9.5</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1505,19 +2351,34 @@
         <v>1</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.55</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="5"/>
+        <v>4.55</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="6"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1534,19 +2395,34 @@
         <v>1</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="M12" s="3">
+        <v>2</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="5"/>
+        <v>8.4</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="6"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1563,19 +2439,34 @@
         <v>1</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1592,19 +2483,34 @@
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
+        <v>4</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1621,19 +2527,34 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.75</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1647,7 +2568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>20</v>
       </c>
@@ -1656,18 +2577,33 @@
         <v>80.790000000000006</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" ref="I17:J17" si="4">SUM(I2:I15)</f>
+        <f t="shared" ref="I17:J17" si="8">SUM(I2:I15)</f>
         <v>86.539999999999992</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>100.28999999999999</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="4">
+        <f>SUM(O2:O15)</f>
+        <v>167.87</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" ref="P17:Q17" si="9">SUM(P2:P15)</f>
+        <v>211.17000000000002</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="9"/>
+        <v>211.42000000000002</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H17:J17">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
     <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
highlighted the highest and smallest amount paid by tim
</commit_message>
<xml_diff>
--- a/work_book_1.xlsx
+++ b/work_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70641D3D-497A-4E62-8612-5DA268394882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE486342-F52E-464B-93EE-6B6D49535EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74BCC72C-4CB7-45E2-B286-F8BEF58EF335}"/>
   </bookViews>
@@ -179,7 +179,77 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1511,16 +1581,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1556,7 +1626,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8915400" y="1724025"/>
+              <a:off x="4076700" y="457200"/>
               <a:ext cx="4267200" cy="2352675"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1890,7 +1960,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H19" activeCellId="1" sqref="O17:Q17 H19"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,8 +2672,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H17:J17">
+    <cfRule type="top10" dxfId="6" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:Q17">
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
     <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>